<commit_message>
3/19/18 capture work and std util configs
</commit_message>
<xml_diff>
--- a/CurrentWork_Delta/RoughTestCalculationsCXTA.xlsx
+++ b/CurrentWork_Delta/RoughTestCalculationsCXTA.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mark\CurrentWork_home\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mark\CurrentWork_Delta\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="408" windowWidth="20160" windowHeight="9204"/>
+    <workbookView xWindow="0" yWindow="816" windowWidth="20160" windowHeight="9204"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Min Low</t>
   </si>
@@ -40,21 +40,12 @@
     <t>Percent</t>
   </si>
   <si>
-    <t>Min</t>
-  </si>
-  <si>
     <t>#of Test</t>
   </si>
   <si>
     <t>% of TC</t>
   </si>
   <si>
-    <t>Min/ run</t>
-  </si>
-  <si>
-    <t>total Min</t>
-  </si>
-  <si>
     <t>Total Hrs</t>
   </si>
   <si>
@@ -73,22 +64,40 @@
     <t>Second High</t>
   </si>
   <si>
-    <t>Sec / run</t>
-  </si>
-  <si>
-    <t>total Sec</t>
-  </si>
-  <si>
     <t>Total Min</t>
   </si>
   <si>
     <t>Hours</t>
   </si>
   <si>
-    <t>Sec / Test</t>
-  </si>
-  <si>
     <t># of Test</t>
+  </si>
+  <si>
+    <t>Min Per</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>Test Run</t>
+  </si>
+  <si>
+    <t>3 Test Runs</t>
+  </si>
+  <si>
+    <t>Sec per</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Sec </t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Min</t>
   </si>
 </sst>
 </file>
@@ -119,7 +128,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -128,11 +137,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thick">
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
+      <top style="thick">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -141,7 +150,7 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
+      <top style="thick">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -149,17 +158,17 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thick">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thick">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thick">
         <color indexed="64"/>
       </left>
       <right/>
@@ -169,7 +178,7 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thick">
         <color indexed="64"/>
       </right>
       <top/>
@@ -177,12 +186,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thick">
         <color indexed="64"/>
       </left>
       <right/>
       <top/>
-      <bottom style="medium">
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -191,13 +200,39 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -211,15 +246,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -227,11 +265,13 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -513,21 +553,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I17"/>
+  <dimension ref="B1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="7.88671875" style="1" customWidth="1"/>
+    <col min="3" max="5" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="10.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="1"/>
     <col min="8" max="8" width="10" style="1" customWidth="1"/>
     <col min="9" max="9" width="11.109375" style="1" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B2" s="14"/>
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -541,7 +587,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="15"/>
       <c r="D3" s="1">
         <v>3</v>
       </c>
@@ -559,123 +606,130 @@
       </c>
     </row>
     <row r="4" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="3">
+    <row r="5" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5">
         <v>475</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="7" t="s">
+      <c r="H6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="6">
+      <c r="B7" s="8">
         <f>H3</f>
         <v>0.5</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="3">
         <f>B5*B7</f>
         <v>237.5</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="3">
         <f>D3</f>
         <v>3</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="3">
         <f>C7*D7</f>
         <v>712.5</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="9" t="s">
-        <v>10</v>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="10" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="6">
+      <c r="B8" s="8">
         <f>I3</f>
         <v>0.25</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="3">
         <f>B5*B8</f>
         <v>118.75</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="3">
         <f>E3</f>
         <v>7</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="3">
         <f>C8*D8</f>
         <v>831.25</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="9"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="10"/>
     </row>
     <row r="9" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="10">
+      <c r="B9" s="11">
         <f>I3</f>
         <v>0.25</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="12">
         <f>B5*B9</f>
         <v>118.75</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="12">
         <f>F3</f>
         <v>12</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="12">
         <f>C9*D9</f>
         <v>1425</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="12">
         <f>SUM(E7:E9)</f>
         <v>2968.75</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="12">
         <f>F9/60</f>
         <v>49.479166666666664</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="13">
         <f>G9/10</f>
         <v>4.9479166666666661</v>
       </c>
     </row>
+    <row r="10" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D11" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>3</v>
@@ -701,111 +755,125 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="3">
+    <row r="13" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="5">
         <v>600</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="7" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="7" t="s">
+      <c r="G13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="E14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="F14" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="G14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="6">
+      <c r="B15" s="8">
         <f>G12</f>
         <v>0.5</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="3">
         <f>B13*B15</f>
         <v>300</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="3">
         <f>D12</f>
         <v>5</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="3">
         <f>C15*D15</f>
         <v>1500</v>
       </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="9"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="10"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="6">
+      <c r="B16" s="8">
         <f>H12</f>
         <v>0.3</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="3">
         <f>B13*B16</f>
         <v>180</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="3">
         <f>E12</f>
         <v>15</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="3">
         <f>C16*D16</f>
         <v>2700</v>
       </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="10">
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="10"/>
+    </row>
+    <row r="17" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="11">
         <f>I12</f>
         <v>0.2</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="12">
         <f>B13*B17</f>
         <v>120</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="12">
         <f>F12</f>
         <v>30</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="12">
         <f>C17*D17</f>
         <v>3600</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="12">
         <f>SUM(E15:E17)</f>
         <v>7800</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="12">
         <f>F17/60</f>
         <v>130</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="13">
         <f>G17/60</f>
         <v>2.1666666666666665</v>
       </c>
+    </row>
+    <row r="18" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I19" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
4/4/18 some new files come mods in other files
</commit_message>
<xml_diff>
--- a/CurrentWork_Delta/RoughTestCalculationsCXTA.xlsx
+++ b/CurrentWork_Delta/RoughTestCalculationsCXTA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="816" windowWidth="20160" windowHeight="9204"/>
+    <workbookView xWindow="0" yWindow="1224" windowWidth="20160" windowHeight="9204"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>Min Low</t>
   </si>
@@ -46,15 +46,6 @@
     <t>% of TC</t>
   </si>
   <si>
-    <t>Total Hrs</t>
-  </si>
-  <si>
-    <t>Days</t>
-  </si>
-  <si>
-    <t>10 hr Staff</t>
-  </si>
-  <si>
     <t>Second Low</t>
   </si>
   <si>
@@ -64,18 +55,12 @@
     <t>Second High</t>
   </si>
   <si>
-    <t>Total Min</t>
-  </si>
-  <si>
     <t>Hours</t>
   </si>
   <si>
     <t># of Test</t>
   </si>
   <si>
-    <t>Min Per</t>
-  </si>
-  <si>
     <t>Test Case</t>
   </si>
   <si>
@@ -98,6 +83,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Min</t>
+  </si>
+  <si>
+    <t>Total Sec</t>
+  </si>
+  <si>
+    <t>Sec Per</t>
   </si>
 </sst>
 </file>
@@ -246,32 +237,75 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -566,14 +600,14 @@
     <col min="3" max="5" width="8.88671875" style="1"/>
     <col min="6" max="6" width="10.21875" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" style="1"/>
-    <col min="8" max="8" width="10" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="11.109375" style="1" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="14"/>
+      <c r="B2" s="7"/>
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -588,15 +622,15 @@
       </c>
     </row>
     <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="15"/>
+      <c r="B3" s="8"/>
       <c r="D3" s="1">
-        <v>3</v>
+        <v>180</v>
       </c>
       <c r="E3" s="1">
-        <v>7</v>
+        <v>420</v>
       </c>
       <c r="F3" s="1">
-        <v>12</v>
+        <v>720</v>
       </c>
       <c r="H3" s="1">
         <v>0.5</v>
@@ -607,133 +641,136 @@
     </row>
     <row r="4" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>475</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="7"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="25" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="D6" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>8</v>
+      <c r="H6" s="26" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="8">
-        <f>H3</f>
+      <c r="B7" s="10">
         <v>0.5</v>
       </c>
-      <c r="C7" s="3">
-        <f>B5*B7</f>
-        <v>237.5</v>
-      </c>
-      <c r="D7" s="3">
+      <c r="C7" s="12">
+        <v>238</v>
+      </c>
+      <c r="D7" s="12">
         <f>D3</f>
-        <v>3</v>
-      </c>
-      <c r="E7" s="3">
+        <v>180</v>
+      </c>
+      <c r="E7" s="12">
         <f>C7*D7</f>
-        <v>712.5</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="10" t="s">
-        <v>7</v>
-      </c>
+        <v>42840</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="13"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="8">
+      <c r="B8" s="10">
         <f>I3</f>
         <v>0.25</v>
       </c>
-      <c r="C8" s="3">
-        <f>B5*B8</f>
-        <v>118.75</v>
-      </c>
-      <c r="D8" s="3">
+      <c r="C8" s="12">
+        <v>118</v>
+      </c>
+      <c r="D8" s="12">
         <f>E3</f>
-        <v>7</v>
-      </c>
-      <c r="E8" s="3">
+        <v>420</v>
+      </c>
+      <c r="E8" s="12">
         <f>C8*D8</f>
-        <v>831.25</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="10"/>
+        <v>49560</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="11">
+      <c r="B9" s="14">
         <f>I3</f>
         <v>0.25</v>
       </c>
-      <c r="C9" s="12">
-        <f>B5*B9</f>
-        <v>118.75</v>
-      </c>
-      <c r="D9" s="12">
+      <c r="C9" s="15">
+        <v>119</v>
+      </c>
+      <c r="D9" s="15">
         <f>F3</f>
-        <v>12</v>
-      </c>
-      <c r="E9" s="12">
+        <v>720</v>
+      </c>
+      <c r="E9" s="15">
         <f>C9*D9</f>
-        <v>1425</v>
-      </c>
-      <c r="F9" s="12">
+        <v>85680</v>
+      </c>
+      <c r="F9" s="15">
         <f>SUM(E7:E9)</f>
-        <v>2968.75</v>
-      </c>
-      <c r="G9" s="12">
+        <v>178080</v>
+      </c>
+      <c r="G9" s="15">
         <f>F9/60</f>
-        <v>49.479166666666664</v>
-      </c>
-      <c r="H9" s="13">
-        <f>G9/10</f>
-        <v>4.9479166666666661</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+        <v>2968</v>
+      </c>
+      <c r="H9" s="24">
+        <f>G9/60</f>
+        <v>49.466666666666669</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+    </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D11" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="27" t="s">
         <v>3</v>
       </c>
+      <c r="H11" s="27"/>
     </row>
     <row r="12" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D12" s="1">
@@ -742,13 +779,13 @@
       <c r="E12" s="1">
         <v>15</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="27">
         <v>30</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="27">
         <v>0.5</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="27">
         <v>0.3</v>
       </c>
       <c r="I12" s="1">
@@ -756,124 +793,124 @@
       </c>
     </row>
     <row r="13" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>600</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="6" t="s">
+      <c r="C13" s="5"/>
+      <c r="D13" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>21</v>
+      <c r="F13" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H14" s="17" t="s">
-        <v>13</v>
+      <c r="H14" s="26" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="8">
+      <c r="B15" s="16">
         <f>G12</f>
         <v>0.5</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="17">
         <f>B13*B15</f>
         <v>300</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="17">
         <f>D12</f>
         <v>5</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="17">
         <f>C15*D15</f>
         <v>1500</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="10"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="18"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="8">
+      <c r="B16" s="16">
         <f>H12</f>
         <v>0.3</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="17">
         <f>B13*B16</f>
         <v>180</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="17">
         <f>E12</f>
         <v>15</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="17">
         <f>C16*D16</f>
         <v>2700</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="10"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="18"/>
     </row>
     <row r="17" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="11">
+      <c r="B17" s="19">
         <f>I12</f>
         <v>0.2</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="20">
         <f>B13*B17</f>
         <v>120</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="20">
         <f>F12</f>
         <v>30</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="20">
         <f>C17*D17</f>
         <v>3600</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="20">
         <f>SUM(E15:E17)</f>
         <v>7800</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="20">
         <f>F17/60</f>
         <v>130</v>
       </c>
-      <c r="H17" s="13">
+      <c r="H17" s="21">
         <f>G17/60</f>
         <v>2.1666666666666665</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="I19" s="16"/>
+      <c r="I19" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
4/10/18 revision on excel and pics.  mods to slides
</commit_message>
<xml_diff>
--- a/CurrentWork_Delta/RoughTestCalculationsCXTA.xlsx
+++ b/CurrentWork_Delta/RoughTestCalculationsCXTA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1224" windowWidth="20160" windowHeight="9204"/>
+    <workbookView xWindow="0" yWindow="1632" windowWidth="20160" windowHeight="9204"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>Min Low</t>
   </si>
@@ -43,9 +43,6 @@
     <t>#of Test</t>
   </si>
   <si>
-    <t>% of TC</t>
-  </si>
-  <si>
     <t>Second Low</t>
   </si>
   <si>
@@ -61,18 +58,12 @@
     <t># of Test</t>
   </si>
   <si>
-    <t>Test Case</t>
-  </si>
-  <si>
     <t>Test Run</t>
   </si>
   <si>
     <t>3 Test Runs</t>
   </si>
   <si>
-    <t>Sec per</t>
-  </si>
-  <si>
     <t xml:space="preserve">Total Sec </t>
   </si>
   <si>
@@ -88,7 +79,28 @@
     <t>Total Sec</t>
   </si>
   <si>
-    <t>Sec Per</t>
+    <t>1/2</t>
+  </si>
+  <si>
+    <t>1/4</t>
+  </si>
+  <si>
+    <t>1/3</t>
+  </si>
+  <si>
+    <t>1/5</t>
+  </si>
+  <si>
+    <t>Per Test</t>
+  </si>
+  <si>
+    <t>Seconds</t>
+  </si>
+  <si>
+    <t>Manual  Cases 475</t>
+  </si>
+  <si>
+    <t>Auto    Cases  600</t>
   </si>
 </sst>
 </file>
@@ -237,22 +249,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -262,22 +268,13 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -305,6 +302,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -590,7 +605,7 @@
   <dimension ref="B1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,7 +622,7 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="7"/>
+      <c r="B2" s="4"/>
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
@@ -622,7 +637,7 @@
       </c>
     </row>
     <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="8"/>
+      <c r="B3" s="5"/>
       <c r="D3" s="1">
         <v>180</v>
       </c>
@@ -641,136 +656,132 @@
     </row>
     <row r="4" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="4">
-        <v>475</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="22" t="s">
+      <c r="B5" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="25" t="s">
-        <v>16</v>
+      <c r="H5" s="18" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="6" t="s">
-        <v>5</v>
-      </c>
+      <c r="B6" s="25"/>
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="26" t="s">
-        <v>9</v>
+      <c r="G6" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="C7" s="12">
+      <c r="B7" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="8">
         <v>238</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="8">
         <f>D3</f>
         <v>180</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="8">
         <f>C7*D7</f>
         <v>42840</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="13"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="10">
-        <f>I3</f>
-        <v>0.25</v>
-      </c>
-      <c r="C8" s="12">
+      <c r="B8" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="8">
         <v>118</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="8">
         <f>E3</f>
         <v>420</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="8">
         <f>C8*D8</f>
         <v>49560</v>
       </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="13"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="14">
-        <f>I3</f>
-        <v>0.25</v>
-      </c>
-      <c r="C9" s="15">
+      <c r="B9" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="10">
         <v>119</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="10">
         <f>F3</f>
         <v>720</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="10">
         <f>C9*D9</f>
         <v>85680</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="10">
         <f>SUM(E7:E9)</f>
         <v>178080</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="10">
         <f>F9/60</f>
         <v>2968</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="17">
         <f>G9/60</f>
         <v>49.466666666666669</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="H11" s="27"/>
+      <c r="H11" s="20"/>
     </row>
     <row r="12" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D12" s="1">
@@ -779,13 +790,13 @@
       <c r="E12" s="1">
         <v>15</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="20">
         <v>30</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="20">
         <v>0.5</v>
       </c>
-      <c r="H12" s="27">
+      <c r="H12" s="20">
         <v>0.3</v>
       </c>
       <c r="I12" s="1">
@@ -793,124 +804,113 @@
       </c>
     </row>
     <row r="13" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="4">
-        <v>600</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="22" t="s">
+      <c r="B13" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="22" t="s">
+      <c r="H13" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="25"/>
+      <c r="C14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="H14" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="6" t="s">
+      <c r="C15" s="11">
+        <v>300</v>
+      </c>
+      <c r="D15" s="11">
         <v>5</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="16">
-        <f>G12</f>
-        <v>0.5</v>
-      </c>
-      <c r="C15" s="17">
-        <f>B13*B15</f>
-        <v>300</v>
-      </c>
-      <c r="D15" s="17">
-        <f>D12</f>
-        <v>5</v>
-      </c>
-      <c r="E15" s="17">
+      <c r="E15" s="11">
         <f>C15*D15</f>
         <v>1500</v>
       </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="18"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="12"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="16">
-        <f>H12</f>
-        <v>0.3</v>
-      </c>
-      <c r="C16" s="17">
-        <f>B13*B16</f>
+      <c r="B16" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="11">
         <v>180</v>
       </c>
-      <c r="D16" s="17">
-        <f>E12</f>
+      <c r="D16" s="11">
         <v>15</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="11">
         <f>C16*D16</f>
         <v>2700</v>
       </c>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="18"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="12"/>
     </row>
     <row r="17" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="19">
-        <f>I12</f>
-        <v>0.2</v>
-      </c>
-      <c r="C17" s="20">
-        <f>B13*B17</f>
+      <c r="B17" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="13">
         <v>120</v>
       </c>
-      <c r="D17" s="20">
-        <f>F12</f>
+      <c r="D17" s="13">
         <v>30</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="13">
         <f>C17*D17</f>
         <v>3600</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F17" s="13">
         <f>SUM(E15:E17)</f>
         <v>7800</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="13">
         <f>F17/60</f>
         <v>130</v>
       </c>
-      <c r="H17" s="21">
+      <c r="H17" s="14">
         <f>G17/60</f>
         <v>2.1666666666666665</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="I19" s="9"/>
+      <c r="I19" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>